<commit_message>
modified:   update overtime in Overtime.xml
</commit_message>
<xml_diff>
--- a/残業.xlsx
+++ b/残業.xlsx
@@ -835,14 +835,14 @@
         <v>42552</v>
       </c>
       <c r="B11">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C11">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.93333333333333335</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -856,15 +856,15 @@
       </c>
       <c r="H11" s="1">
         <f t="shared" si="2"/>
-        <v>26.933333333333334</v>
+        <v>29.566666666666666</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="4"/>
-        <v>158.51666666666668</v>
+        <v>161.15</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="3"/>
-        <v>48978.641666666677</v>
+        <v>53668.608333333337</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -885,7 +885,7 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="4"/>
-        <v>158.51666666666668</v>
+        <v>161.15</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="3"/>
@@ -910,7 +910,7 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="4"/>
-        <v>158.51666666666668</v>
+        <v>161.15</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" si="3"/>
@@ -925,7 +925,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="6">
         <f>SUM(J2:J13)</f>
-        <v>283728.14166666666</v>
+        <v>288418.10833333334</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
overtime.xml at home 2016/07/31 00:00
</commit_message>
<xml_diff>
--- a/残業.xlsx
+++ b/残業.xlsx
@@ -85,14 +85,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -100,7 +100,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:J155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -835,36 +835,36 @@
         <v>42552</v>
       </c>
       <c r="B11">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C11">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.56666666666666665</v>
+        <v>0.15</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>0.95</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="2"/>
-        <v>29.566666666666666</v>
+        <v>34.15</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="4"/>
-        <v>161.15</v>
+        <v>165.73333333333335</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="3"/>
-        <v>53668.608333333337</v>
+        <v>62373.816666666658</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -885,7 +885,7 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="4"/>
-        <v>161.15</v>
+        <v>165.73333333333335</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="3"/>
@@ -910,7 +910,7 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="4"/>
-        <v>161.15</v>
+        <v>165.73333333333335</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" si="3"/>
@@ -925,7 +925,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="6">
         <f>SUM(J2:J13)</f>
-        <v>288418.10833333334</v>
+        <v>297123.31666666665</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>